<commit_message>
took meat out of obj. func, took credit and contract out of model structure
</commit_message>
<xml_diff>
--- a/dairyclimatemodel/data/model_data.xlsx
+++ b/dairyclimatemodel/data/model_data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\GitHub\household_ghg_model\household_ghg_model\dairyclimatemodel\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{44FA5150-F5A1-44D4-8908-A1C64AD8A554}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="898" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752" tabRatio="898" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="7" r:id="rId1"/>
@@ -624,7 +630,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -1018,32 +1024,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>1</v>
       </c>
@@ -1054,7 +1060,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1074,7 +1080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1094,7 +1100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1114,7 +1120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1134,7 +1140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1154,7 +1160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
         <v>0</v>
       </c>
@@ -1174,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1194,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1214,7 +1220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1234,7 +1240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1254,7 +1260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1274,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
         <v>0</v>
       </c>
@@ -1294,7 +1300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="11:16" ht="15" x14ac:dyDescent="0.3">
       <c r="K19" t="s">
         <v>0</v>
       </c>
@@ -1320,14 +1326,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="24"/>
@@ -1394,14 +1400,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1450,14 +1456,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1505,7 +1511,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V148"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -1515,15 +1521,15 @@
       <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="24" customWidth="1"/>
-    <col min="2" max="11" width="8.85546875" style="24"/>
-    <col min="12" max="12" width="10.42578125" style="24" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="24"/>
+    <col min="1" max="1" width="14.88671875" style="24" customWidth="1"/>
+    <col min="2" max="11" width="8.88671875" style="24"/>
+    <col min="12" max="12" width="10.44140625" style="24" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D1" s="24" t="s">
         <v>57</v>
       </c>
@@ -1558,7 +1564,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
         <v>41</v>
       </c>
@@ -1602,7 +1608,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>70</v>
       </c>
@@ -1644,7 +1650,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>81</v>
       </c>
@@ -1686,7 +1692,7 @@
       <c r="Q4" s="5"/>
       <c r="R4" s="8"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>80</v>
       </c>
@@ -1726,7 +1732,7 @@
       </c>
       <c r="N5" s="17"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>78</v>
       </c>
@@ -1765,7 +1771,7 @@
       </c>
       <c r="N6" s="17"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
         <v>79</v>
       </c>
@@ -1808,7 +1814,7 @@
       <c r="S7" s="8"/>
       <c r="T7" s="8"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
         <v>77</v>
       </c>
@@ -1842,7 +1848,7 @@
       <c r="O8" s="2"/>
       <c r="R8" s="8"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="str">
         <f t="shared" ref="A9:A20" si="1">A3</f>
         <v>adultf_loc</v>
@@ -1885,7 +1891,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="str">
         <f t="shared" si="1"/>
         <v>youngm_loc</v>
@@ -1936,7 +1942,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="str">
         <f t="shared" si="1"/>
         <v>youngf_loc</v>
@@ -1988,7 +1994,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="str">
         <f t="shared" si="1"/>
         <v>weanerm_loc</v>
@@ -2031,7 +2037,7 @@
       <c r="N12" s="19"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="str">
         <f t="shared" si="1"/>
         <v>weanerf_loc</v>
@@ -2075,7 +2081,7 @@
       <c r="O13" s="2"/>
       <c r="S13" s="15"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="str">
         <f t="shared" si="1"/>
         <v>reprod_loc</v>
@@ -2109,7 +2115,7 @@
       <c r="N14" s="17"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="str">
         <f t="shared" si="1"/>
         <v>adultf_loc</v>
@@ -2159,7 +2165,7 @@
         <v>5.081967213114754</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="str">
         <f t="shared" si="1"/>
         <v>youngm_loc</v>
@@ -2211,7 +2217,7 @@
         <v>7.2131147540983607</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="str">
         <f t="shared" si="1"/>
         <v>youngf_loc</v>
@@ -2257,7 +2263,7 @@
       <c r="N17" s="17"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="str">
         <f t="shared" si="1"/>
         <v>weanerm_loc</v>
@@ -2300,7 +2306,7 @@
       <c r="N18" s="17"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="str">
         <f t="shared" si="1"/>
         <v>weanerf_loc</v>
@@ -2343,7 +2349,7 @@
       <c r="N19" s="17"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="str">
         <f t="shared" si="1"/>
         <v>reprod_loc</v>
@@ -2382,7 +2388,7 @@
       <c r="N20" s="17"/>
       <c r="O20" s="2"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>71</v>
       </c>
@@ -2423,7 +2429,7 @@
       </c>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>76</v>
       </c>
@@ -2464,7 +2470,7 @@
       <c r="N22" s="17"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>75</v>
       </c>
@@ -2505,7 +2511,7 @@
       <c r="N23" s="17"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>73</v>
       </c>
@@ -2545,7 +2551,7 @@
       <c r="N24" s="17"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>74</v>
       </c>
@@ -2585,7 +2591,7 @@
       <c r="N25" s="17"/>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
         <v>72</v>
       </c>
@@ -2618,7 +2624,7 @@
       <c r="N26" s="17"/>
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="str">
         <f t="shared" ref="A27:A38" si="4">A21</f>
         <v>adultf_imp</v>
@@ -2660,7 +2666,7 @@
       </c>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="str">
         <f t="shared" si="4"/>
         <v>youngm_imp</v>
@@ -2705,7 +2711,7 @@
       <c r="N28" s="17"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="str">
         <f t="shared" si="4"/>
         <v>youngf_imp</v>
@@ -2750,7 +2756,7 @@
       <c r="N29" s="17"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="str">
         <f t="shared" si="4"/>
         <v>weanerm_imp</v>
@@ -2792,7 +2798,7 @@
       <c r="N30" s="19"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="str">
         <f t="shared" si="4"/>
         <v>weanerf_imp</v>
@@ -2834,7 +2840,7 @@
       <c r="N31" s="17"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="str">
         <f t="shared" si="4"/>
         <v>reprod_imp</v>
@@ -2867,7 +2873,7 @@
       <c r="N32" s="17"/>
       <c r="O32" s="2"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="24" t="str">
         <f t="shared" si="4"/>
         <v>adultf_imp</v>
@@ -2909,7 +2915,7 @@
       </c>
       <c r="O33" s="2"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="str">
         <f t="shared" si="4"/>
         <v>youngm_imp</v>
@@ -2954,7 +2960,7 @@
       <c r="N34" s="17"/>
       <c r="O34" s="2"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="24" t="str">
         <f t="shared" si="4"/>
         <v>youngf_imp</v>
@@ -2999,7 +3005,7 @@
       <c r="N35" s="17"/>
       <c r="O35" s="2"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="24" t="str">
         <f t="shared" si="4"/>
         <v>weanerm_imp</v>
@@ -3041,7 +3047,7 @@
       <c r="N36" s="17"/>
       <c r="O36" s="2"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="24" t="str">
         <f t="shared" si="4"/>
         <v>weanerf_imp</v>
@@ -3083,7 +3089,7 @@
       <c r="N37" s="17"/>
       <c r="O37" s="2"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="24" t="str">
         <f t="shared" si="4"/>
         <v>reprod_imp</v>
@@ -3121,7 +3127,7 @@
       <c r="N38" s="17"/>
       <c r="O38" s="2"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G39" s="12"/>
       <c r="H39" s="14"/>
       <c r="I39" s="12"/>
@@ -3131,7 +3137,7 @@
       <c r="N39" s="12"/>
       <c r="O39" s="2"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G40" s="12"/>
       <c r="H40" s="14"/>
       <c r="I40" s="12"/>
@@ -3141,7 +3147,7 @@
       <c r="N40" s="12"/>
       <c r="O40" s="2"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G41" s="12"/>
       <c r="H41" s="14"/>
       <c r="I41" s="12"/>
@@ -3151,7 +3157,7 @@
       <c r="N41" s="12"/>
       <c r="O41" s="2"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G42" s="12"/>
       <c r="H42" s="14"/>
       <c r="I42" s="12"/>
@@ -3161,7 +3167,7 @@
       <c r="N42" s="12"/>
       <c r="O42" s="2"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D43" s="24" t="s">
         <v>82</v>
       </c>
@@ -3174,7 +3180,7 @@
       <c r="N43" s="12"/>
       <c r="O43" s="2"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D44" s="24" t="s">
         <v>109</v>
       </c>
@@ -3193,7 +3199,7 @@
       <c r="N44" s="12"/>
       <c r="O44" s="2"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D45" s="24" t="s">
         <v>110</v>
       </c>
@@ -3212,7 +3218,7 @@
       <c r="N45" s="12"/>
       <c r="O45" s="2"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D46" s="24" t="s">
         <v>111</v>
       </c>
@@ -3231,7 +3237,7 @@
       <c r="N46" s="12"/>
       <c r="O46" s="2"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D47" s="24" t="s">
         <v>184</v>
       </c>
@@ -3246,7 +3252,7 @@
       <c r="N47" s="12"/>
       <c r="O47" s="2"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D48" s="24" t="s">
         <v>183</v>
       </c>
@@ -3261,7 +3267,7 @@
       <c r="N48" s="12"/>
       <c r="O48" s="2"/>
     </row>
-    <row r="49" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D49" s="24" t="s">
         <v>83</v>
       </c>
@@ -3276,7 +3282,7 @@
       <c r="N49" s="12"/>
       <c r="O49" s="2"/>
     </row>
-    <row r="50" spans="4:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D50" s="24" t="s">
         <v>182</v>
       </c>
@@ -3291,7 +3297,7 @@
       <c r="N50" s="12"/>
       <c r="O50" s="2"/>
     </row>
-    <row r="51" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D51" s="24" t="s">
         <v>181</v>
       </c>
@@ -3306,7 +3312,7 @@
       <c r="N51" s="12"/>
       <c r="O51" s="2"/>
     </row>
-    <row r="52" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D52" s="24" t="s">
         <v>185</v>
       </c>
@@ -3321,7 +3327,7 @@
       <c r="N52" s="12"/>
       <c r="O52" s="2"/>
     </row>
-    <row r="53" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D53" s="24" t="s">
         <v>186</v>
       </c>
@@ -3336,7 +3342,7 @@
       <c r="N53" s="12"/>
       <c r="O53" s="2"/>
     </row>
-    <row r="54" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D54" s="24" t="s">
         <v>187</v>
       </c>
@@ -3351,7 +3357,7 @@
       <c r="N54" s="12"/>
       <c r="O54" s="2"/>
     </row>
-    <row r="55" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D55" s="24" t="s">
         <v>188</v>
       </c>
@@ -3366,7 +3372,7 @@
       <c r="N55" s="12"/>
       <c r="O55" s="2"/>
     </row>
-    <row r="56" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:15" x14ac:dyDescent="0.3">
       <c r="G56" s="17"/>
       <c r="H56" s="14"/>
       <c r="I56" s="12"/>
@@ -3376,7 +3382,7 @@
       <c r="N56" s="12"/>
       <c r="O56" s="2"/>
     </row>
-    <row r="57" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:15" x14ac:dyDescent="0.3">
       <c r="G57" s="12"/>
       <c r="H57" s="14"/>
       <c r="I57" s="12"/>
@@ -3386,7 +3392,7 @@
       <c r="N57" s="12"/>
       <c r="O57" s="2"/>
     </row>
-    <row r="58" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:15" x14ac:dyDescent="0.3">
       <c r="G58" s="12"/>
       <c r="H58" s="14"/>
       <c r="I58" s="12"/>
@@ -3396,7 +3402,7 @@
       <c r="N58" s="12"/>
       <c r="O58" s="2"/>
     </row>
-    <row r="59" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:15" x14ac:dyDescent="0.3">
       <c r="G59" s="12"/>
       <c r="H59" s="14"/>
       <c r="I59" s="12"/>
@@ -3406,7 +3412,7 @@
       <c r="N59" s="12"/>
       <c r="O59" s="2"/>
     </row>
-    <row r="60" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:15" x14ac:dyDescent="0.3">
       <c r="G60" s="12"/>
       <c r="H60" s="14"/>
       <c r="I60" s="12"/>
@@ -3416,7 +3422,7 @@
       <c r="N60" s="12"/>
       <c r="O60" s="2"/>
     </row>
-    <row r="61" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:15" x14ac:dyDescent="0.3">
       <c r="G61" s="12"/>
       <c r="H61" s="14"/>
       <c r="I61" s="12"/>
@@ -3426,7 +3432,7 @@
       <c r="N61" s="12"/>
       <c r="O61" s="2"/>
     </row>
-    <row r="62" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:15" x14ac:dyDescent="0.3">
       <c r="G62" s="12"/>
       <c r="H62" s="14"/>
       <c r="I62" s="12"/>
@@ -3436,7 +3442,7 @@
       <c r="N62" s="12"/>
       <c r="O62" s="2"/>
     </row>
-    <row r="63" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:15" x14ac:dyDescent="0.3">
       <c r="G63" s="12"/>
       <c r="H63" s="14"/>
       <c r="I63" s="12"/>
@@ -3446,7 +3452,7 @@
       <c r="N63" s="12"/>
       <c r="O63" s="2"/>
     </row>
-    <row r="64" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:15" x14ac:dyDescent="0.3">
       <c r="G64" s="12"/>
       <c r="H64" s="14"/>
       <c r="I64" s="12"/>
@@ -3456,7 +3462,7 @@
       <c r="N64" s="12"/>
       <c r="O64" s="2"/>
     </row>
-    <row r="65" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="7:15" x14ac:dyDescent="0.3">
       <c r="G65" s="12"/>
       <c r="H65" s="14"/>
       <c r="I65" s="12"/>
@@ -3466,7 +3472,7 @@
       <c r="N65" s="12"/>
       <c r="O65" s="2"/>
     </row>
-    <row r="66" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:15" x14ac:dyDescent="0.3">
       <c r="G66" s="12"/>
       <c r="H66" s="14"/>
       <c r="I66" s="12"/>
@@ -3476,7 +3482,7 @@
       <c r="N66" s="12"/>
       <c r="O66" s="2"/>
     </row>
-    <row r="67" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="7:15" x14ac:dyDescent="0.3">
       <c r="G67" s="12"/>
       <c r="H67" s="14"/>
       <c r="I67" s="12"/>
@@ -3486,7 +3492,7 @@
       <c r="N67" s="12"/>
       <c r="O67" s="2"/>
     </row>
-    <row r="68" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="7:15" x14ac:dyDescent="0.3">
       <c r="G68" s="12"/>
       <c r="H68" s="14"/>
       <c r="I68" s="12"/>
@@ -3496,7 +3502,7 @@
       <c r="N68" s="12"/>
       <c r="O68" s="2"/>
     </row>
-    <row r="69" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="7:15" x14ac:dyDescent="0.3">
       <c r="G69" s="12"/>
       <c r="H69" s="14"/>
       <c r="I69" s="12"/>
@@ -3506,7 +3512,7 @@
       <c r="N69" s="12"/>
       <c r="O69" s="2"/>
     </row>
-    <row r="70" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="7:15" x14ac:dyDescent="0.3">
       <c r="G70" s="12"/>
       <c r="H70" s="14"/>
       <c r="I70" s="12"/>
@@ -3516,7 +3522,7 @@
       <c r="N70" s="12"/>
       <c r="O70" s="2"/>
     </row>
-    <row r="71" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="7:15" x14ac:dyDescent="0.3">
       <c r="G71" s="12"/>
       <c r="H71" s="14"/>
       <c r="I71" s="12"/>
@@ -3526,7 +3532,7 @@
       <c r="N71" s="12"/>
       <c r="O71" s="2"/>
     </row>
-    <row r="72" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="7:15" x14ac:dyDescent="0.3">
       <c r="G72" s="12"/>
       <c r="H72" s="14"/>
       <c r="I72" s="12"/>
@@ -3536,7 +3542,7 @@
       <c r="N72" s="12"/>
       <c r="O72" s="2"/>
     </row>
-    <row r="73" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="7:15" x14ac:dyDescent="0.3">
       <c r="G73" s="12"/>
       <c r="H73" s="14"/>
       <c r="I73" s="12"/>
@@ -3546,7 +3552,7 @@
       <c r="N73" s="12"/>
       <c r="O73" s="2"/>
     </row>
-    <row r="74" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="7:15" x14ac:dyDescent="0.3">
       <c r="G74" s="12"/>
       <c r="H74" s="14"/>
       <c r="I74" s="12"/>
@@ -3556,7 +3562,7 @@
       <c r="N74" s="12"/>
       <c r="O74" s="2"/>
     </row>
-    <row r="75" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="7:15" x14ac:dyDescent="0.3">
       <c r="G75" s="12"/>
       <c r="H75" s="14"/>
       <c r="I75" s="12"/>
@@ -3566,7 +3572,7 @@
       <c r="N75" s="12"/>
       <c r="O75" s="2"/>
     </row>
-    <row r="76" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="7:15" x14ac:dyDescent="0.3">
       <c r="G76" s="12"/>
       <c r="H76" s="14"/>
       <c r="I76" s="12"/>
@@ -3576,10 +3582,10 @@
       <c r="N76" s="12"/>
       <c r="O76" s="2"/>
     </row>
-    <row r="77" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="7:15" x14ac:dyDescent="0.3">
       <c r="O77" s="2"/>
     </row>
-    <row r="95" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G95" s="14"/>
       <c r="H95" s="14"/>
       <c r="I95" s="12"/>
@@ -3588,7 +3594,7 @@
       <c r="M95" s="4"/>
       <c r="N95" s="12"/>
     </row>
-    <row r="96" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="G96" s="14"/>
@@ -3599,7 +3605,7 @@
       <c r="M96" s="4"/>
       <c r="N96" s="12"/>
     </row>
-    <row r="97" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
       <c r="G97" s="14"/>
@@ -3610,7 +3616,7 @@
       <c r="M97" s="4"/>
       <c r="N97" s="12"/>
     </row>
-    <row r="98" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G98" s="14"/>
       <c r="H98" s="14"/>
       <c r="I98" s="12"/>
@@ -3619,7 +3625,7 @@
       <c r="M98" s="4"/>
       <c r="N98" s="12"/>
     </row>
-    <row r="99" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G99" s="14"/>
       <c r="H99" s="14"/>
       <c r="I99" s="12"/>
@@ -3628,7 +3634,7 @@
       <c r="M99" s="4"/>
       <c r="N99" s="12"/>
     </row>
-    <row r="100" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G100" s="14"/>
       <c r="H100" s="14"/>
       <c r="I100" s="12"/>
@@ -3637,7 +3643,7 @@
       <c r="M100" s="4"/>
       <c r="N100" s="12"/>
     </row>
-    <row r="101" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G101" s="12"/>
       <c r="H101" s="14"/>
       <c r="I101" s="12"/>
@@ -3646,7 +3652,7 @@
       <c r="M101" s="4"/>
       <c r="N101" s="12"/>
     </row>
-    <row r="102" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G102" s="12"/>
       <c r="H102" s="14"/>
       <c r="I102" s="12"/>
@@ -3655,7 +3661,7 @@
       <c r="M102" s="4"/>
       <c r="N102" s="12"/>
     </row>
-    <row r="103" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G103" s="12"/>
       <c r="H103" s="14"/>
       <c r="I103" s="12"/>
@@ -3664,7 +3670,7 @@
       <c r="M103" s="4"/>
       <c r="N103" s="12"/>
     </row>
-    <row r="104" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G104" s="12"/>
       <c r="H104" s="14"/>
       <c r="I104" s="12"/>
@@ -3673,7 +3679,7 @@
       <c r="M104" s="4"/>
       <c r="N104" s="12"/>
     </row>
-    <row r="105" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G105" s="12"/>
       <c r="H105" s="14"/>
       <c r="I105" s="12"/>
@@ -3682,7 +3688,7 @@
       <c r="M105" s="4"/>
       <c r="N105" s="12"/>
     </row>
-    <row r="106" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G106" s="12"/>
       <c r="H106" s="14"/>
       <c r="I106" s="12"/>
@@ -3691,7 +3697,7 @@
       <c r="M106" s="4"/>
       <c r="N106" s="12"/>
     </row>
-    <row r="107" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G107" s="12"/>
       <c r="H107" s="14"/>
       <c r="I107" s="12"/>
@@ -3700,7 +3706,7 @@
       <c r="M107" s="4"/>
       <c r="N107" s="12"/>
     </row>
-    <row r="108" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G108" s="12"/>
       <c r="H108" s="14"/>
       <c r="I108" s="12"/>
@@ -3709,7 +3715,7 @@
       <c r="M108" s="4"/>
       <c r="N108" s="12"/>
     </row>
-    <row r="109" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G109" s="12"/>
       <c r="H109" s="14"/>
       <c r="I109" s="12"/>
@@ -3718,7 +3724,7 @@
       <c r="M109" s="4"/>
       <c r="N109" s="12"/>
     </row>
-    <row r="110" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G110" s="12"/>
       <c r="H110" s="14"/>
       <c r="I110" s="12"/>
@@ -3727,7 +3733,7 @@
       <c r="M110" s="4"/>
       <c r="N110" s="12"/>
     </row>
-    <row r="111" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G111" s="12"/>
       <c r="H111" s="14"/>
       <c r="I111" s="12"/>
@@ -3736,7 +3742,7 @@
       <c r="M111" s="4"/>
       <c r="N111" s="12"/>
     </row>
-    <row r="112" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="4:14" x14ac:dyDescent="0.3">
       <c r="G112" s="12"/>
       <c r="H112" s="14"/>
       <c r="I112" s="12"/>
@@ -3745,7 +3751,7 @@
       <c r="M112" s="4"/>
       <c r="N112" s="12"/>
     </row>
-    <row r="113" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G113" s="12"/>
       <c r="H113" s="14"/>
       <c r="I113" s="12"/>
@@ -3754,7 +3760,7 @@
       <c r="M113" s="4"/>
       <c r="N113" s="12"/>
     </row>
-    <row r="114" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="114" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G114" s="12"/>
       <c r="H114" s="14"/>
       <c r="I114" s="12"/>
@@ -3763,7 +3769,7 @@
       <c r="M114" s="4"/>
       <c r="N114" s="12"/>
     </row>
-    <row r="115" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="115" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G115" s="12"/>
       <c r="H115" s="14"/>
       <c r="I115" s="12"/>
@@ -3772,7 +3778,7 @@
       <c r="M115" s="4"/>
       <c r="N115" s="12"/>
     </row>
-    <row r="116" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="116" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G116" s="12"/>
       <c r="H116" s="14"/>
       <c r="I116" s="12"/>
@@ -3781,7 +3787,7 @@
       <c r="M116" s="4"/>
       <c r="N116" s="12"/>
     </row>
-    <row r="117" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="117" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G117" s="12"/>
       <c r="H117" s="14"/>
       <c r="I117" s="12"/>
@@ -3790,7 +3796,7 @@
       <c r="M117" s="4"/>
       <c r="N117" s="12"/>
     </row>
-    <row r="118" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="118" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G118" s="12"/>
       <c r="H118" s="14"/>
       <c r="I118" s="12"/>
@@ -3799,7 +3805,7 @@
       <c r="M118" s="4"/>
       <c r="N118" s="12"/>
     </row>
-    <row r="119" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="119" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G119" s="12"/>
       <c r="H119" s="14"/>
       <c r="I119" s="12"/>
@@ -3808,7 +3814,7 @@
       <c r="M119" s="4"/>
       <c r="N119" s="12"/>
     </row>
-    <row r="120" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="120" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G120" s="12"/>
       <c r="H120" s="14"/>
       <c r="I120" s="12"/>
@@ -3817,7 +3823,7 @@
       <c r="M120" s="4"/>
       <c r="N120" s="12"/>
     </row>
-    <row r="121" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="121" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G121" s="12"/>
       <c r="H121" s="14"/>
       <c r="I121" s="12"/>
@@ -3826,7 +3832,7 @@
       <c r="M121" s="4"/>
       <c r="N121" s="12"/>
     </row>
-    <row r="122" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="122" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G122" s="12"/>
       <c r="H122" s="14"/>
       <c r="I122" s="12"/>
@@ -3835,7 +3841,7 @@
       <c r="M122" s="4"/>
       <c r="N122" s="12"/>
     </row>
-    <row r="123" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="123" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G123" s="12"/>
       <c r="H123" s="14"/>
       <c r="I123" s="12"/>
@@ -3844,7 +3850,7 @@
       <c r="M123" s="4"/>
       <c r="N123" s="12"/>
     </row>
-    <row r="124" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="124" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G124" s="12"/>
       <c r="H124" s="14"/>
       <c r="I124" s="12"/>
@@ -3853,7 +3859,7 @@
       <c r="M124" s="4"/>
       <c r="N124" s="12"/>
     </row>
-    <row r="125" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="125" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G125" s="12"/>
       <c r="H125" s="14"/>
       <c r="I125" s="12"/>
@@ -3862,7 +3868,7 @@
       <c r="M125" s="4"/>
       <c r="N125" s="12"/>
     </row>
-    <row r="126" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="126" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G126" s="12"/>
       <c r="H126" s="14"/>
       <c r="I126" s="12"/>
@@ -3871,7 +3877,7 @@
       <c r="M126" s="4"/>
       <c r="N126" s="12"/>
     </row>
-    <row r="127" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="127" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G127" s="12"/>
       <c r="H127" s="14"/>
       <c r="I127" s="12"/>
@@ -3880,7 +3886,7 @@
       <c r="M127" s="4"/>
       <c r="N127" s="12"/>
     </row>
-    <row r="128" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="128" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G128" s="12"/>
       <c r="H128" s="14"/>
       <c r="I128" s="12"/>
@@ -3889,7 +3895,7 @@
       <c r="M128" s="4"/>
       <c r="N128" s="12"/>
     </row>
-    <row r="129" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="129" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G129" s="12"/>
       <c r="H129" s="14"/>
       <c r="I129" s="12"/>
@@ -3898,7 +3904,7 @@
       <c r="M129" s="4"/>
       <c r="N129" s="12"/>
     </row>
-    <row r="130" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="130" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G130" s="12"/>
       <c r="H130" s="14"/>
       <c r="I130" s="12"/>
@@ -3907,7 +3913,7 @@
       <c r="M130" s="4"/>
       <c r="N130" s="12"/>
     </row>
-    <row r="131" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="131" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G131" s="12"/>
       <c r="H131" s="14"/>
       <c r="I131" s="12"/>
@@ -3916,7 +3922,7 @@
       <c r="M131" s="4"/>
       <c r="N131" s="12"/>
     </row>
-    <row r="132" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="132" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G132" s="12"/>
       <c r="H132" s="14"/>
       <c r="I132" s="12"/>
@@ -3925,7 +3931,7 @@
       <c r="M132" s="4"/>
       <c r="N132" s="12"/>
     </row>
-    <row r="133" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="133" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G133" s="12"/>
       <c r="H133" s="14"/>
       <c r="I133" s="12"/>
@@ -3934,7 +3940,7 @@
       <c r="M133" s="4"/>
       <c r="N133" s="12"/>
     </row>
-    <row r="134" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="134" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G134" s="12"/>
       <c r="H134" s="14"/>
       <c r="I134" s="12"/>
@@ -3943,7 +3949,7 @@
       <c r="M134" s="4"/>
       <c r="N134" s="12"/>
     </row>
-    <row r="135" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="135" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G135" s="12"/>
       <c r="H135" s="14"/>
       <c r="I135" s="12"/>
@@ -3952,7 +3958,7 @@
       <c r="M135" s="4"/>
       <c r="N135" s="12"/>
     </row>
-    <row r="136" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="136" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G136" s="12"/>
       <c r="H136" s="14"/>
       <c r="I136" s="12"/>
@@ -3961,7 +3967,7 @@
       <c r="M136" s="4"/>
       <c r="N136" s="12"/>
     </row>
-    <row r="137" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="137" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G137" s="12"/>
       <c r="H137" s="14"/>
       <c r="I137" s="12"/>
@@ -3970,7 +3976,7 @@
       <c r="M137" s="4"/>
       <c r="N137" s="12"/>
     </row>
-    <row r="138" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="138" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G138" s="12"/>
       <c r="H138" s="14"/>
       <c r="I138" s="12"/>
@@ -3979,7 +3985,7 @@
       <c r="M138" s="4"/>
       <c r="N138" s="12"/>
     </row>
-    <row r="139" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="139" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G139" s="12"/>
       <c r="H139" s="14"/>
       <c r="I139" s="12"/>
@@ -3988,7 +3994,7 @@
       <c r="M139" s="4"/>
       <c r="N139" s="12"/>
     </row>
-    <row r="140" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="140" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G140" s="12"/>
       <c r="H140" s="14"/>
       <c r="I140" s="12"/>
@@ -3997,7 +4003,7 @@
       <c r="M140" s="4"/>
       <c r="N140" s="12"/>
     </row>
-    <row r="141" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="141" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G141" s="12"/>
       <c r="H141" s="14"/>
       <c r="I141" s="12"/>
@@ -4006,7 +4012,7 @@
       <c r="M141" s="4"/>
       <c r="N141" s="12"/>
     </row>
-    <row r="142" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="142" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G142" s="12"/>
       <c r="H142" s="14"/>
       <c r="I142" s="12"/>
@@ -4015,7 +4021,7 @@
       <c r="M142" s="4"/>
       <c r="N142" s="12"/>
     </row>
-    <row r="143" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="143" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G143" s="12"/>
       <c r="H143" s="14"/>
       <c r="I143" s="12"/>
@@ -4024,7 +4030,7 @@
       <c r="M143" s="4"/>
       <c r="N143" s="12"/>
     </row>
-    <row r="144" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="144" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G144" s="12"/>
       <c r="H144" s="14"/>
       <c r="I144" s="12"/>
@@ -4033,7 +4039,7 @@
       <c r="M144" s="4"/>
       <c r="N144" s="12"/>
     </row>
-    <row r="145" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="145" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G145" s="12"/>
       <c r="H145" s="14"/>
       <c r="I145" s="12"/>
@@ -4042,7 +4048,7 @@
       <c r="M145" s="4"/>
       <c r="N145" s="12"/>
     </row>
-    <row r="146" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="146" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G146" s="12"/>
       <c r="H146" s="14"/>
       <c r="I146" s="12"/>
@@ -4051,7 +4057,7 @@
       <c r="M146" s="4"/>
       <c r="N146" s="12"/>
     </row>
-    <row r="147" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="147" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G147" s="12"/>
       <c r="H147" s="14"/>
       <c r="I147" s="12"/>
@@ -4060,7 +4066,7 @@
       <c r="M147" s="4"/>
       <c r="N147" s="12"/>
     </row>
-    <row r="148" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="148" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G148" s="12"/>
       <c r="H148" s="14"/>
       <c r="I148" s="12"/>
@@ -4076,16 +4082,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E1" t="s">
         <v>153</v>
       </c>
@@ -4096,7 +4102,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -4111,7 +4117,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -4120,7 +4126,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -4129,7 +4135,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -4138,7 +4144,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -4147,7 +4153,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -4156,7 +4162,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4165,7 +4171,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -4174,7 +4180,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -4183,7 +4189,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -4192,7 +4198,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -4201,7 +4207,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -4216,24 +4222,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -4273,7 +4279,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -4332,7 +4338,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -4387,7 +4393,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -4437,7 +4443,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -4490,7 +4496,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -4557,7 +4563,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -4604,7 +4610,7 @@
         <v>0.17899999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>119</v>
       </c>
@@ -4651,7 +4657,7 @@
         <v>0.61399999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>158</v>
       </c>
@@ -4698,7 +4704,7 @@
         <v>0.42499999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>195</v>
       </c>
@@ -4745,7 +4751,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="15" x14ac:dyDescent="0.3">
       <c r="H12" t="s">
         <v>196</v>
       </c>
@@ -4758,37 +4764,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="F2" r:id="rId3"/>
-    <hyperlink ref="E2" r:id="rId4"/>
-    <hyperlink ref="G2" r:id="rId5"/>
-    <hyperlink ref="I2" r:id="rId6"/>
-    <hyperlink ref="J2" r:id="rId7"/>
-    <hyperlink ref="K2" r:id="rId8"/>
-    <hyperlink ref="O2" r:id="rId9"/>
-    <hyperlink ref="M2" r:id="rId10"/>
-    <hyperlink ref="B2" r:id="rId11"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="G2" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="I2" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="J2" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="K2" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="O2" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="M2" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
+    <hyperlink ref="B2" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="5" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C1" s="27" t="s">
         <v>108</v>
       </c>
@@ -4798,7 +4804,7 @@
       <c r="G1" s="27"/>
       <c r="H1" s="27"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -4842,7 +4848,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C3" s="4" t="s">
         <v>33</v>
       </c>
@@ -4880,7 +4886,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -4930,7 +4936,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -4986,7 +4992,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -5042,7 +5048,7 @@
         <v>3.4624999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -5098,7 +5104,7 @@
         <v>13.85</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -5148,7 +5154,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -5198,7 +5204,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -5248,7 +5254,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -5307,7 +5313,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -5366,7 +5372,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -5425,7 +5431,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -5484,7 +5490,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -5534,7 +5540,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f>A4</f>
         <v>m01</v>
@@ -5585,7 +5591,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f t="shared" ref="A17:A39" si="7">A5</f>
         <v>m02</v>
@@ -5636,7 +5642,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f t="shared" si="7"/>
         <v>m03</v>
@@ -5687,7 +5693,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f t="shared" si="7"/>
         <v>m04</v>
@@ -5738,7 +5744,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f t="shared" si="7"/>
         <v>m05</v>
@@ -5789,7 +5795,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f t="shared" si="7"/>
         <v>m06</v>
@@ -5840,7 +5846,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f t="shared" si="7"/>
         <v>m07</v>
@@ -5891,7 +5897,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f t="shared" si="7"/>
         <v>m08</v>
@@ -5942,7 +5948,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f t="shared" si="7"/>
         <v>m09</v>
@@ -5993,7 +5999,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f t="shared" si="7"/>
         <v>m10</v>
@@ -6044,7 +6050,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f t="shared" si="7"/>
         <v>m11</v>
@@ -6095,7 +6101,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f t="shared" si="7"/>
         <v>m12</v>
@@ -6146,7 +6152,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f t="shared" si="7"/>
         <v>m01</v>
@@ -6197,7 +6203,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f t="shared" si="7"/>
         <v>m02</v>
@@ -6248,7 +6254,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f t="shared" si="7"/>
         <v>m03</v>
@@ -6299,7 +6305,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f t="shared" si="7"/>
         <v>m04</v>
@@ -6350,7 +6356,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f t="shared" si="7"/>
         <v>m05</v>
@@ -6401,7 +6407,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f t="shared" si="7"/>
         <v>m06</v>
@@ -6452,7 +6458,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f t="shared" si="7"/>
         <v>m07</v>
@@ -6503,7 +6509,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f t="shared" si="7"/>
         <v>m08</v>
@@ -6554,7 +6560,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f t="shared" si="7"/>
         <v>m09</v>
@@ -6605,7 +6611,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f t="shared" si="7"/>
         <v>m10</v>
@@ -6656,7 +6662,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f t="shared" si="7"/>
         <v>m11</v>
@@ -6707,7 +6713,7 @@
         <v>9.8928571428571423</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f t="shared" si="7"/>
         <v>m12</v>
@@ -6768,19 +6774,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N10" sqref="N10:P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -6794,7 +6800,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -6815,7 +6821,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -6836,7 +6842,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -6854,7 +6860,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -6875,7 +6881,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -6896,7 +6902,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -6914,7 +6920,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -6931,7 +6937,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -6948,7 +6954,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -6980,7 +6986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -7014,7 +7020,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -7040,7 +7046,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>86</v>
       </c>
@@ -7066,7 +7072,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>86</v>
       </c>
@@ -7083,7 +7089,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -7100,7 +7106,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -7117,7 +7123,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -7134,7 +7140,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -7151,7 +7157,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -7168,7 +7174,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>86</v>
       </c>
@@ -7185,7 +7191,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -7202,7 +7208,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -7219,7 +7225,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>86</v>
       </c>
@@ -7236,7 +7242,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -7253,7 +7259,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -7270,7 +7276,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>86</v>
       </c>
@@ -7287,7 +7293,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -7304,7 +7310,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>86</v>
       </c>
@@ -7321,7 +7327,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -7338,7 +7344,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>86</v>
       </c>
@@ -7355,7 +7361,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -7372,7 +7378,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -7389,7 +7395,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>86</v>
       </c>
@@ -7406,7 +7412,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>86</v>
       </c>
@@ -7423,7 +7429,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -7440,7 +7446,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>86</v>
       </c>
@@ -7457,7 +7463,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -7474,7 +7480,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>165</v>
       </c>
@@ -7492,7 +7498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>165</v>
       </c>
@@ -7510,7 +7516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>165</v>
       </c>
@@ -7528,7 +7534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>165</v>
       </c>
@@ -7546,7 +7552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>165</v>
       </c>
@@ -7564,7 +7570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>165</v>
       </c>
@@ -7582,7 +7588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>165</v>
       </c>
@@ -7599,7 +7605,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>165</v>
       </c>
@@ -7616,7 +7622,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>165</v>
       </c>
@@ -7633,7 +7639,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>165</v>
       </c>
@@ -7650,7 +7656,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>165</v>
       </c>
@@ -7667,7 +7673,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>165</v>
       </c>
@@ -7684,7 +7690,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>165</v>
       </c>
@@ -7701,7 +7707,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>165</v>
       </c>
@@ -7718,7 +7724,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>165</v>
       </c>
@@ -7735,7 +7741,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>165</v>
       </c>
@@ -7752,7 +7758,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>165</v>
       </c>
@@ -7769,7 +7775,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>165</v>
       </c>
@@ -7786,7 +7792,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>165</v>
       </c>
@@ -7803,7 +7809,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>165</v>
       </c>
@@ -7820,7 +7826,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>165</v>
       </c>
@@ -7837,7 +7843,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>165</v>
       </c>
@@ -7854,7 +7860,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>165</v>
       </c>
@@ -7871,7 +7877,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>165</v>
       </c>
@@ -7888,7 +7894,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>165</v>
       </c>
@@ -7905,7 +7911,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>165</v>
       </c>
@@ -7922,7 +7928,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>165</v>
       </c>
@@ -7939,7 +7945,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>165</v>
       </c>
@@ -7956,7 +7962,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>165</v>
       </c>
@@ -7973,7 +7979,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>165</v>
       </c>
@@ -7990,7 +7996,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>165</v>
       </c>
@@ -8007,7 +8013,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>165</v>
       </c>
@@ -8024,7 +8030,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>165</v>
       </c>
@@ -8041,7 +8047,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>165</v>
       </c>
@@ -8058,7 +8064,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>165</v>
       </c>
@@ -8075,7 +8081,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>165</v>
       </c>
@@ -8092,7 +8098,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>171</v>
       </c>
@@ -8110,7 +8116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>171</v>
       </c>
@@ -8128,7 +8134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>171</v>
       </c>
@@ -8146,7 +8152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>171</v>
       </c>
@@ -8164,7 +8170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>171</v>
       </c>
@@ -8182,7 +8188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>171</v>
       </c>
@@ -8200,7 +8206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>171</v>
       </c>
@@ -8217,7 +8223,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>171</v>
       </c>
@@ -8234,7 +8240,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>171</v>
       </c>
@@ -8251,7 +8257,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>171</v>
       </c>
@@ -8268,7 +8274,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>171</v>
       </c>
@@ -8285,7 +8291,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>171</v>
       </c>
@@ -8302,7 +8308,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>171</v>
       </c>
@@ -8319,7 +8325,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>171</v>
       </c>
@@ -8336,7 +8342,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>171</v>
       </c>
@@ -8353,7 +8359,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>171</v>
       </c>
@@ -8370,7 +8376,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>171</v>
       </c>
@@ -8387,7 +8393,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>171</v>
       </c>
@@ -8404,7 +8410,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>171</v>
       </c>
@@ -8421,7 +8427,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>171</v>
       </c>
@@ -8438,7 +8444,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>171</v>
       </c>
@@ -8455,7 +8461,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>171</v>
       </c>
@@ -8472,7 +8478,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>171</v>
       </c>
@@ -8489,7 +8495,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>171</v>
       </c>
@@ -8506,7 +8512,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>171</v>
       </c>
@@ -8523,7 +8529,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>171</v>
       </c>
@@ -8540,7 +8546,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>171</v>
       </c>
@@ -8557,7 +8563,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>171</v>
       </c>
@@ -8574,7 +8580,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>171</v>
       </c>
@@ -8591,7 +8597,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>171</v>
       </c>
@@ -8608,7 +8614,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>171</v>
       </c>
@@ -8625,7 +8631,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>171</v>
       </c>
@@ -8642,7 +8648,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>171</v>
       </c>
@@ -8659,7 +8665,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>171</v>
       </c>
@@ -8676,7 +8682,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>171</v>
       </c>
@@ -8693,7 +8699,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>171</v>
       </c>
@@ -8710,7 +8716,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>172</v>
       </c>
@@ -8728,7 +8734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>172</v>
       </c>
@@ -8746,7 +8752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>172</v>
       </c>
@@ -8764,7 +8770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>172</v>
       </c>
@@ -8782,7 +8788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>172</v>
       </c>
@@ -8800,7 +8806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>172</v>
       </c>
@@ -8818,7 +8824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>172</v>
       </c>
@@ -8835,7 +8841,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>172</v>
       </c>
@@ -8852,7 +8858,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>172</v>
       </c>
@@ -8869,7 +8875,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>172</v>
       </c>
@@ -8886,7 +8892,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>172</v>
       </c>
@@ -8903,7 +8909,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>172</v>
       </c>
@@ -8920,7 +8926,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>172</v>
       </c>
@@ -8937,7 +8943,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>172</v>
       </c>
@@ -8954,7 +8960,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>172</v>
       </c>
@@ -8971,7 +8977,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>172</v>
       </c>
@@ -8988,7 +8994,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>172</v>
       </c>
@@ -9005,7 +9011,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>172</v>
       </c>
@@ -9022,7 +9028,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>172</v>
       </c>
@@ -9039,7 +9045,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>172</v>
       </c>
@@ -9056,7 +9062,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>172</v>
       </c>
@@ -9073,7 +9079,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>172</v>
       </c>
@@ -9090,7 +9096,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>172</v>
       </c>
@@ -9107,7 +9113,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>172</v>
       </c>
@@ -9124,7 +9130,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>172</v>
       </c>
@@ -9141,7 +9147,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>172</v>
       </c>
@@ -9158,7 +9164,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>172</v>
       </c>
@@ -9175,7 +9181,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>172</v>
       </c>
@@ -9192,7 +9198,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>172</v>
       </c>
@@ -9209,7 +9215,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>172</v>
       </c>
@@ -9226,7 +9232,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>172</v>
       </c>
@@ -9243,7 +9249,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>172</v>
       </c>
@@ -9260,7 +9266,7 @@
         <v>5600.0000000000009</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>172</v>
       </c>
@@ -9277,7 +9283,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>172</v>
       </c>
@@ -9294,7 +9300,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>172</v>
       </c>
@@ -9311,7 +9317,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>172</v>
       </c>
@@ -9335,20 +9341,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="11" max="11" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="11" max="11" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>90</v>
       </c>
@@ -9368,7 +9374,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -9388,7 +9394,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>80</v>
       </c>
@@ -9412,7 +9418,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>78</v>
       </c>
@@ -9447,7 +9453,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>79</v>
       </c>
@@ -9479,7 +9485,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>70</v>
       </c>
@@ -9492,7 +9498,7 @@
         <v>122004</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>77</v>
       </c>
@@ -9505,7 +9511,7 @@
         <v>122004</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
@@ -9516,7 +9522,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>75</v>
       </c>
@@ -9527,7 +9533,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>73</v>
       </c>
@@ -9546,7 +9552,7 @@
         <v>135560</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>74</v>
       </c>
@@ -9565,7 +9571,7 @@
         <v>135560</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>71</v>
       </c>
@@ -9584,7 +9590,7 @@
         <v>135560</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>72</v>
       </c>
@@ -9603,7 +9609,7 @@
         <v>135560</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>81</v>
       </c>
@@ -9614,7 +9620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>80</v>
       </c>
@@ -9625,7 +9631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>78</v>
       </c>
@@ -9638,7 +9644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>79</v>
       </c>
@@ -9653,7 +9659,7 @@
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
     </row>
-    <row r="18" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>88</v>
       </c>
@@ -9666,7 +9672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>70</v>
       </c>
@@ -9679,7 +9685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
@@ -9690,7 +9696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>75</v>
       </c>
@@ -9705,7 +9711,7 @@
         <v>866.66666666666663</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>73</v>
       </c>
@@ -9719,7 +9725,7 @@
       </c>
       <c r="K22" s="21"/>
     </row>
-    <row r="23" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
@@ -9732,7 +9738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>89</v>
       </c>
@@ -9745,7 +9751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
@@ -9758,10 +9764,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>98</v>
       </c>
@@ -9799,7 +9805,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>0</v>
       </c>
@@ -9844,24 +9850,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -9878,7 +9884,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -9895,7 +9901,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -9912,7 +9918,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -9929,7 +9935,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -9946,7 +9952,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -9963,7 +9969,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -9980,7 +9986,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -9997,7 +10003,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -10014,7 +10020,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -10031,7 +10037,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>78</v>
       </c>
@@ -10048,7 +10054,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -10065,7 +10071,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -10088,16 +10094,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>17</v>
       </c>
@@ -10135,7 +10141,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>144</v>
       </c>
@@ -10176,7 +10182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>145</v>
       </c>
@@ -10217,7 +10223,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -10258,7 +10264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>146</v>
       </c>
@@ -10299,7 +10305,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>147</v>
       </c>
@@ -10340,7 +10346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>148</v>
       </c>
@@ -10381,7 +10387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>161</v>
       </c>
@@ -10422,7 +10428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>144</v>
       </c>
@@ -10463,7 +10469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>145</v>
       </c>
@@ -10504,7 +10510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
         <v>147</v>
       </c>
@@ -10545,7 +10551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
         <v>189</v>
       </c>
@@ -10586,7 +10592,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
         <v>148</v>
       </c>
@@ -10627,7 +10633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
         <v>190</v>
       </c>
@@ -10668,7 +10674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
         <v>197</v>
       </c>
@@ -10709,7 +10715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
         <v>128</v>
       </c>
@@ -10750,7 +10756,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>161</v>
       </c>
@@ -10791,7 +10797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="24"/>
       <c r="B33" s="24"/>
       <c r="C33" s="24"/>

</xml_diff>